<commit_message>
Added some result files
</commit_message>
<xml_diff>
--- a/Result/Before_SRSE_with_different_Standard_Deviations/Threshold values for IEEE 30 and 118 bus systems.xlsx
+++ b/Result/Before_SRSE_with_different_Standard_Deviations/Threshold values for IEEE 30 and 118 bus systems.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iitbacin-my.sharepoint.com/personal/214070018_iitb_ac_in/Documents/Desktop/SRSE_Simulation/Result/Before_SRSE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iitbacin-my.sharepoint.com/personal/214070018_iitb_ac_in/Documents/Desktop/SRSE_Simulation/Result/Before_SRSE_with_different_Standard_Deviations/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="62" documentId="8_{9FEF018B-079F-460B-AAC4-378BD35482E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{636CE056-FEBA-4E6A-9BB2-97B81E4F467B}"/>
@@ -293,43 +293,43 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -350,6 +350,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -651,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91DB520-EF87-49BE-A1E1-8A2641DD2740}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,61 +666,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6" t="s">
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="7"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="12"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="3">
         <v>0.7</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>0.9</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>0.99</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>0.7</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>0.9</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>0.99</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <v>0.7</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="3">
         <v>0.9</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="4">
         <v>0.99</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -746,12 +750,12 @@
       <c r="J3" s="1">
         <v>0.22013074159622201</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="5">
         <v>0.243034407496452</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
@@ -779,12 +783,12 @@
       <c r="J4" s="1">
         <v>1.1000453233718901</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="5">
         <v>1.22773349285126</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
@@ -812,12 +816,12 @@
       <c r="J5" s="1">
         <v>2.2020568847656299</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="5">
         <v>2.3735146522521999</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -847,12 +851,12 @@
       <c r="J6" s="2">
         <v>0.118028752505779</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="6">
         <v>0.123036235570908</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
@@ -880,40 +884,40 @@
       <c r="J7" s="2">
         <v>0.58770984411239602</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="6">
         <v>0.61595678329467796</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="7">
         <v>327.89343261718801</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="7">
         <v>347.26885986328102</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="7">
         <v>373.40664672851602</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="7">
         <v>1.02661657333374</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="7">
         <v>1.0567277669906601</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="7">
         <v>1.0960602760314899</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="7">
         <v>1.1370724439621001</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="7">
         <v>1.1736855506896999</v>
       </c>
-      <c r="K8" s="16">
+      <c r="K8" s="8">
         <v>1.2195293903350799</v>
       </c>
     </row>
@@ -928,5 +932,6 @@
     <mergeCell ref="A3:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>